<commit_message>
Gannt Modified and Requirements Complete
Made some changes to the Gannt to include extra designs for the system which I missed originally. Following this i completed the Requirements (func/non-func), which i may modify and add to over the next few days.
</commit_message>
<xml_diff>
--- a/Documentation/Gannt.xlsx
+++ b/Documentation/Gannt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Github\Year2\COMP3000-Computing-Project\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Github\Year3\COMP3000-Computing-Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B56001-1A4B-4015-8DC8-1A1A891B7296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D74F453-9226-461C-97E9-7E6C55E71662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>Project start:</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Create Web Dashboard</t>
   </si>
   <si>
-    <t>Script to parse PostgreSQL outputs to web dash</t>
-  </si>
-  <si>
     <t>Security and Evaluation</t>
   </si>
   <si>
@@ -240,6 +237,30 @@
   </si>
   <si>
     <t>Portfolio</t>
+  </si>
+  <si>
+    <t>Functional and Non-Functional Requirements</t>
+  </si>
+  <si>
+    <t>User Stories and Use Cases</t>
+  </si>
+  <si>
+    <t>Wireframes (Low Fidelity)</t>
+  </si>
+  <si>
+    <t>User Flow Diagram</t>
+  </si>
+  <si>
+    <t>System Architecture Diagram</t>
+  </si>
+  <si>
+    <t>Data Flow Diagram (DFD)</t>
+  </si>
+  <si>
+    <t>Entity Relationship Diagram (ERD)</t>
+  </si>
+  <si>
+    <t>API to parse PostgreSQL outputs to web dash</t>
   </si>
 </sst>
 </file>
@@ -252,8 +273,8 @@
     <numFmt numFmtId="166" formatCode="ddd\,\ m/d/yyyy"/>
     <numFmt numFmtId="167" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="168" formatCode="d"/>
-    <numFmt numFmtId="171" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="172" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="169" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="170" formatCode="d/m/yy;@"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -1003,6 +1024,131 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="3" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="3" borderId="7" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="4" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="5" borderId="8" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="10" borderId="9" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="9" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="13" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="13" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="14" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="14" borderId="9" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="17" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1012,135 +1158,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="171" fontId="24" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="171" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="17" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="16" fillId="3" borderId="6" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="16" fillId="3" borderId="7" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="16" fillId="4" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="16" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="16" fillId="5" borderId="8" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="16" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="16" fillId="10" borderId="9" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="9" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="13" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="16" fillId="13" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="14" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="16" fillId="14" borderId="9" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1739,10 +1760,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BK50"/>
+  <dimension ref="A1:BK57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A40" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1750,8 +1771,8 @@
     <col min="1" max="1" width="2.69921875" style="11" customWidth="1"/>
     <col min="2" max="2" width="22.69921875" customWidth="1"/>
     <col min="3" max="3" width="10.69921875" customWidth="1"/>
-    <col min="4" max="4" width="10.69921875" style="104" customWidth="1"/>
-    <col min="5" max="5" width="10.69921875" style="105" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" style="88" customWidth="1"/>
+    <col min="5" max="5" width="10.69921875" style="89" customWidth="1"/>
     <col min="6" max="6" width="2.69921875" customWidth="1"/>
     <col min="7" max="7" width="6" hidden="1" customWidth="1"/>
     <col min="8" max="64" width="2.69921875" customWidth="1"/>
@@ -1759,65 +1780,65 @@
   <sheetData>
     <row r="1" spans="1:63" ht="90" customHeight="1" x14ac:dyDescent="1.05">
       <c r="A1" s="12"/>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="64" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="14"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="80"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="66"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="110"/>
+      <c r="N1" s="110"/>
       <c r="O1" s="16"/>
-      <c r="P1" s="77">
+      <c r="P1" s="107">
         <v>45922</v>
       </c>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
+      <c r="Q1" s="108"/>
+      <c r="R1" s="108"/>
+      <c r="S1" s="108"/>
+      <c r="T1" s="108"/>
+      <c r="U1" s="108"/>
+      <c r="V1" s="108"/>
+      <c r="W1" s="108"/>
+      <c r="X1" s="108"/>
+      <c r="Y1" s="108"/>
     </row>
     <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="56" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="15"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="82"/>
-      <c r="H2" s="71" t="s">
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
+      <c r="H2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="69">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
+      <c r="P2" s="105">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="106"/>
+      <c r="X2" s="106"/>
+      <c r="Y2" s="106"/>
     </row>
     <row r="3" spans="1:63" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -1825,342 +1846,342 @@
         <v>2</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="84"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="70"/>
     </row>
     <row r="4" spans="1:63" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="84"/>
-      <c r="H4" s="75">
+      <c r="D4" s="71"/>
+      <c r="E4" s="70"/>
+      <c r="H4" s="102">
         <f>H5</f>
-        <v>45922</v>
-      </c>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73">
+        <v>45936</v>
+      </c>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="100"/>
+      <c r="O4" s="100">
         <f>O5</f>
-        <v>45929</v>
-      </c>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73">
+        <v>45943</v>
+      </c>
+      <c r="P4" s="100"/>
+      <c r="Q4" s="100"/>
+      <c r="R4" s="100"/>
+      <c r="S4" s="100"/>
+      <c r="T4" s="100"/>
+      <c r="U4" s="100"/>
+      <c r="V4" s="100">
         <f>V5</f>
-        <v>45936</v>
-      </c>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="73">
+        <v>45950</v>
+      </c>
+      <c r="W4" s="100"/>
+      <c r="X4" s="100"/>
+      <c r="Y4" s="100"/>
+      <c r="Z4" s="100"/>
+      <c r="AA4" s="100"/>
+      <c r="AB4" s="100"/>
+      <c r="AC4" s="100">
         <f>AC5</f>
-        <v>45943</v>
-      </c>
-      <c r="AD4" s="73"/>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="73">
+        <v>45957</v>
+      </c>
+      <c r="AD4" s="100"/>
+      <c r="AE4" s="100"/>
+      <c r="AF4" s="100"/>
+      <c r="AG4" s="100"/>
+      <c r="AH4" s="100"/>
+      <c r="AI4" s="100"/>
+      <c r="AJ4" s="100">
         <f>AJ5</f>
-        <v>45950</v>
-      </c>
-      <c r="AK4" s="73"/>
-      <c r="AL4" s="73"/>
-      <c r="AM4" s="73"/>
-      <c r="AN4" s="73"/>
-      <c r="AO4" s="73"/>
-      <c r="AP4" s="73"/>
-      <c r="AQ4" s="73">
+        <v>45964</v>
+      </c>
+      <c r="AK4" s="100"/>
+      <c r="AL4" s="100"/>
+      <c r="AM4" s="100"/>
+      <c r="AN4" s="100"/>
+      <c r="AO4" s="100"/>
+      <c r="AP4" s="100"/>
+      <c r="AQ4" s="100">
         <f>AQ5</f>
-        <v>45957</v>
-      </c>
-      <c r="AR4" s="73"/>
-      <c r="AS4" s="73"/>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
-      <c r="AW4" s="73"/>
-      <c r="AX4" s="73">
+        <v>45971</v>
+      </c>
+      <c r="AR4" s="100"/>
+      <c r="AS4" s="100"/>
+      <c r="AT4" s="100"/>
+      <c r="AU4" s="100"/>
+      <c r="AV4" s="100"/>
+      <c r="AW4" s="100"/>
+      <c r="AX4" s="100">
         <f>AX5</f>
-        <v>45964</v>
-      </c>
-      <c r="AY4" s="73"/>
-      <c r="AZ4" s="73"/>
-      <c r="BA4" s="73"/>
-      <c r="BB4" s="73"/>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="73"/>
-      <c r="BE4" s="73">
+        <v>45978</v>
+      </c>
+      <c r="AY4" s="100"/>
+      <c r="AZ4" s="100"/>
+      <c r="BA4" s="100"/>
+      <c r="BB4" s="100"/>
+      <c r="BC4" s="100"/>
+      <c r="BD4" s="100"/>
+      <c r="BE4" s="100">
         <f>BE5</f>
-        <v>45971</v>
-      </c>
-      <c r="BF4" s="73"/>
-      <c r="BG4" s="73"/>
-      <c r="BH4" s="73"/>
-      <c r="BI4" s="73"/>
-      <c r="BJ4" s="73"/>
-      <c r="BK4" s="74"/>
+        <v>45985</v>
+      </c>
+      <c r="BF4" s="100"/>
+      <c r="BG4" s="100"/>
+      <c r="BH4" s="100"/>
+      <c r="BI4" s="100"/>
+      <c r="BJ4" s="100"/>
+      <c r="BK4" s="101"/>
     </row>
     <row r="5" spans="1:63" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="65" t="s">
+      <c r="A5" s="111"/>
+      <c r="B5" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="103" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="21">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45922</v>
+        <v>45936</v>
       </c>
       <c r="I5" s="21">
         <f>H5+1</f>
-        <v>45923</v>
+        <v>45937</v>
       </c>
       <c r="J5" s="21">
         <f t="shared" ref="J5:AW5" si="0">I5+1</f>
-        <v>45924</v>
+        <v>45938</v>
       </c>
       <c r="K5" s="21">
         <f t="shared" si="0"/>
-        <v>45925</v>
+        <v>45939</v>
       </c>
       <c r="L5" s="21">
         <f t="shared" si="0"/>
-        <v>45926</v>
+        <v>45940</v>
       </c>
       <c r="M5" s="21">
         <f t="shared" si="0"/>
-        <v>45927</v>
+        <v>45941</v>
       </c>
       <c r="N5" s="22">
         <f t="shared" si="0"/>
-        <v>45928</v>
+        <v>45942</v>
       </c>
       <c r="O5" s="23">
         <f>N5+1</f>
-        <v>45929</v>
+        <v>45943</v>
       </c>
       <c r="P5" s="21">
         <f>O5+1</f>
-        <v>45930</v>
+        <v>45944</v>
       </c>
       <c r="Q5" s="21">
         <f t="shared" si="0"/>
-        <v>45931</v>
+        <v>45945</v>
       </c>
       <c r="R5" s="21">
         <f t="shared" si="0"/>
-        <v>45932</v>
+        <v>45946</v>
       </c>
       <c r="S5" s="21">
         <f t="shared" si="0"/>
-        <v>45933</v>
+        <v>45947</v>
       </c>
       <c r="T5" s="21">
         <f t="shared" si="0"/>
-        <v>45934</v>
+        <v>45948</v>
       </c>
       <c r="U5" s="22">
         <f t="shared" si="0"/>
-        <v>45935</v>
+        <v>45949</v>
       </c>
       <c r="V5" s="23">
         <f>U5+1</f>
-        <v>45936</v>
+        <v>45950</v>
       </c>
       <c r="W5" s="21">
         <f>V5+1</f>
-        <v>45937</v>
+        <v>45951</v>
       </c>
       <c r="X5" s="21">
         <f t="shared" si="0"/>
-        <v>45938</v>
+        <v>45952</v>
       </c>
       <c r="Y5" s="21">
         <f t="shared" si="0"/>
-        <v>45939</v>
+        <v>45953</v>
       </c>
       <c r="Z5" s="21">
         <f t="shared" si="0"/>
-        <v>45940</v>
+        <v>45954</v>
       </c>
       <c r="AA5" s="21">
         <f t="shared" si="0"/>
-        <v>45941</v>
+        <v>45955</v>
       </c>
       <c r="AB5" s="22">
         <f t="shared" si="0"/>
-        <v>45942</v>
+        <v>45956</v>
       </c>
       <c r="AC5" s="23">
         <f>AB5+1</f>
-        <v>45943</v>
+        <v>45957</v>
       </c>
       <c r="AD5" s="21">
         <f>AC5+1</f>
-        <v>45944</v>
+        <v>45958</v>
       </c>
       <c r="AE5" s="21">
         <f t="shared" si="0"/>
-        <v>45945</v>
+        <v>45959</v>
       </c>
       <c r="AF5" s="21">
         <f t="shared" si="0"/>
-        <v>45946</v>
+        <v>45960</v>
       </c>
       <c r="AG5" s="21">
         <f t="shared" si="0"/>
-        <v>45947</v>
+        <v>45961</v>
       </c>
       <c r="AH5" s="21">
         <f t="shared" si="0"/>
-        <v>45948</v>
+        <v>45962</v>
       </c>
       <c r="AI5" s="22">
         <f t="shared" si="0"/>
-        <v>45949</v>
+        <v>45963</v>
       </c>
       <c r="AJ5" s="23">
         <f>AI5+1</f>
-        <v>45950</v>
+        <v>45964</v>
       </c>
       <c r="AK5" s="21">
         <f>AJ5+1</f>
-        <v>45951</v>
+        <v>45965</v>
       </c>
       <c r="AL5" s="21">
         <f t="shared" si="0"/>
-        <v>45952</v>
+        <v>45966</v>
       </c>
       <c r="AM5" s="21">
         <f t="shared" si="0"/>
-        <v>45953</v>
+        <v>45967</v>
       </c>
       <c r="AN5" s="21">
         <f t="shared" si="0"/>
-        <v>45954</v>
+        <v>45968</v>
       </c>
       <c r="AO5" s="21">
         <f t="shared" si="0"/>
-        <v>45955</v>
+        <v>45969</v>
       </c>
       <c r="AP5" s="22">
         <f t="shared" si="0"/>
-        <v>45956</v>
+        <v>45970</v>
       </c>
       <c r="AQ5" s="23">
         <f>AP5+1</f>
-        <v>45957</v>
+        <v>45971</v>
       </c>
       <c r="AR5" s="21">
         <f>AQ5+1</f>
-        <v>45958</v>
+        <v>45972</v>
       </c>
       <c r="AS5" s="21">
         <f t="shared" si="0"/>
-        <v>45959</v>
+        <v>45973</v>
       </c>
       <c r="AT5" s="21">
         <f t="shared" si="0"/>
-        <v>45960</v>
+        <v>45974</v>
       </c>
       <c r="AU5" s="21">
         <f t="shared" si="0"/>
-        <v>45961</v>
+        <v>45975</v>
       </c>
       <c r="AV5" s="21">
         <f t="shared" si="0"/>
-        <v>45962</v>
+        <v>45976</v>
       </c>
       <c r="AW5" s="22">
         <f t="shared" si="0"/>
-        <v>45963</v>
+        <v>45977</v>
       </c>
       <c r="AX5" s="23">
         <f>AW5+1</f>
-        <v>45964</v>
+        <v>45978</v>
       </c>
       <c r="AY5" s="21">
         <f>AX5+1</f>
-        <v>45965</v>
+        <v>45979</v>
       </c>
       <c r="AZ5" s="21">
         <f t="shared" ref="AZ5:BD5" si="1">AY5+1</f>
-        <v>45966</v>
+        <v>45980</v>
       </c>
       <c r="BA5" s="21">
         <f t="shared" si="1"/>
-        <v>45967</v>
+        <v>45981</v>
       </c>
       <c r="BB5" s="21">
         <f t="shared" si="1"/>
-        <v>45968</v>
+        <v>45982</v>
       </c>
       <c r="BC5" s="21">
         <f t="shared" si="1"/>
-        <v>45969</v>
+        <v>45983</v>
       </c>
       <c r="BD5" s="22">
         <f t="shared" si="1"/>
-        <v>45970</v>
+        <v>45984</v>
       </c>
       <c r="BE5" s="23">
         <f>BD5+1</f>
-        <v>45971</v>
+        <v>45985</v>
       </c>
       <c r="BF5" s="21">
         <f>BE5+1</f>
-        <v>45972</v>
+        <v>45986</v>
       </c>
       <c r="BG5" s="21">
         <f t="shared" ref="BG5:BK5" si="2">BF5+1</f>
-        <v>45973</v>
+        <v>45987</v>
       </c>
       <c r="BH5" s="21">
         <f t="shared" si="2"/>
-        <v>45974</v>
+        <v>45988</v>
       </c>
       <c r="BI5" s="21">
         <f t="shared" si="2"/>
-        <v>45975</v>
+        <v>45989</v>
       </c>
       <c r="BJ5" s="21">
         <f t="shared" si="2"/>
-        <v>45976</v>
+        <v>45990</v>
       </c>
       <c r="BK5" s="21">
         <f t="shared" si="2"/>
-        <v>45977</v>
+        <v>45991</v>
       </c>
     </row>
     <row r="6" spans="1:63" s="18" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="64"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
       <c r="H6" s="24" t="str">
         <f t="shared" ref="H6:AM6" si="3">LEFT(TEXT(H5,"ddd"),1)</f>
         <v>M</v>
@@ -2392,8 +2413,8 @@
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
       <c r="G7" s="18" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
@@ -2463,15 +2484,15 @@
       <c r="C8" s="30">
         <v>1</v>
       </c>
-      <c r="D8" s="89">
+      <c r="D8" s="73">
         <v>45922</v>
       </c>
-      <c r="E8" s="90">
+      <c r="E8" s="74">
         <v>45956</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="3">
-        <f t="shared" ref="G8:G48" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="G8:G55" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>35</v>
       </c>
       <c r="H8" s="31"/>
@@ -2539,11 +2560,11 @@
       <c r="C9" s="34">
         <v>1</v>
       </c>
-      <c r="D9" s="91">
+      <c r="D9" s="75">
         <f>E12</f>
         <v>45940</v>
       </c>
-      <c r="E9" s="91">
+      <c r="E9" s="75">
         <f>D9+2</f>
         <v>45942</v>
       </c>
@@ -2617,11 +2638,11 @@
       <c r="C10" s="37">
         <v>1</v>
       </c>
-      <c r="D10" s="92">
+      <c r="D10" s="76">
         <f>E12</f>
         <v>45940</v>
       </c>
-      <c r="E10" s="92">
+      <c r="E10" s="76">
         <f>D10+2</f>
         <v>45942</v>
       </c>
@@ -2695,11 +2716,11 @@
       <c r="C11" s="37">
         <v>1</v>
       </c>
-      <c r="D11" s="92">
+      <c r="D11" s="76">
         <f>E12</f>
         <v>45940</v>
       </c>
-      <c r="E11" s="92">
+      <c r="E11" s="76">
         <f>D11+2</f>
         <v>45942</v>
       </c>
@@ -2773,10 +2794,10 @@
       <c r="C12" s="37">
         <v>1</v>
       </c>
-      <c r="D12" s="92">
+      <c r="D12" s="76">
         <v>45924</v>
       </c>
-      <c r="E12" s="92">
+      <c r="E12" s="76">
         <f>D12+16</f>
         <v>45940</v>
       </c>
@@ -2850,11 +2871,11 @@
       <c r="C13" s="37">
         <v>1</v>
       </c>
-      <c r="D13" s="92">
+      <c r="D13" s="76">
         <f>D12</f>
         <v>45924</v>
       </c>
-      <c r="E13" s="92">
+      <c r="E13" s="76">
         <f>D13+16</f>
         <v>45940</v>
       </c>
@@ -2925,10 +2946,10 @@
       <c r="C14" s="37">
         <v>1</v>
       </c>
-      <c r="D14" s="92">
+      <c r="D14" s="76">
         <v>45940</v>
       </c>
-      <c r="E14" s="92">
+      <c r="E14" s="76">
         <f>D14+14</f>
         <v>45954</v>
       </c>
@@ -2999,10 +3020,10 @@
       <c r="C15" s="37">
         <v>1</v>
       </c>
-      <c r="D15" s="92">
+      <c r="D15" s="76">
         <v>45940</v>
       </c>
-      <c r="E15" s="92">
+      <c r="E15" s="76">
         <f>D15+2</f>
         <v>45942</v>
       </c>
@@ -3076,10 +3097,10 @@
       <c r="C16" s="40">
         <v>0</v>
       </c>
-      <c r="D16" s="93">
+      <c r="D16" s="77">
         <v>45988</v>
       </c>
-      <c r="E16" s="94">
+      <c r="E16" s="78">
         <v>46006</v>
       </c>
       <c r="F16" s="13"/>
@@ -3090,23 +3111,23 @@
     </row>
     <row r="17" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
-      <c r="B17" s="41" t="s">
-        <v>34</v>
+      <c r="B17" s="91" t="s">
+        <v>62</v>
       </c>
       <c r="C17" s="42">
         <v>0</v>
       </c>
-      <c r="D17" s="95">
-        <v>45964</v>
-      </c>
-      <c r="E17" s="95">
-        <f>D17+2</f>
-        <v>45966</v>
+      <c r="D17" s="79">
+        <v>45968</v>
+      </c>
+      <c r="E17" s="79">
+        <f>D17+1</f>
+        <v>45969</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="3">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H17" s="35"/>
       <c r="I17" s="35"/>
@@ -3166,26 +3187,21 @@
       <c r="BK17" s="35"/>
     </row>
     <row r="18" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="41" t="s">
-        <v>35</v>
+      <c r="A18" s="12"/>
+      <c r="B18" s="91" t="s">
+        <v>63</v>
       </c>
       <c r="C18" s="42">
         <v>0</v>
       </c>
-      <c r="D18" s="95">
-        <f>D17</f>
-        <v>45964</v>
-      </c>
-      <c r="E18" s="95">
-        <f>D17+2</f>
-        <v>45966</v>
+      <c r="D18" s="79">
+        <v>45968</v>
+      </c>
+      <c r="E18" s="79">
+        <v>45970</v>
       </c>
       <c r="F18" s="13"/>
-      <c r="G18" s="3">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
       <c r="J18" s="35"/>
@@ -3198,8 +3214,8 @@
       <c r="Q18" s="35"/>
       <c r="R18" s="35"/>
       <c r="S18" s="35"/>
-      <c r="T18" s="38"/>
-      <c r="U18" s="38"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="35"/>
       <c r="V18" s="35"/>
       <c r="W18" s="35"/>
       <c r="X18" s="35"/>
@@ -3243,26 +3259,22 @@
       <c r="BJ18" s="35"/>
       <c r="BK18" s="35"/>
     </row>
-    <row r="19" spans="1:63" s="32" customFormat="1" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="107" t="s">
-        <v>40</v>
+    <row r="19" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="91" t="s">
+        <v>64</v>
       </c>
       <c r="C19" s="42">
         <v>0</v>
       </c>
-      <c r="D19" s="95">
-        <v>45964</v>
-      </c>
-      <c r="E19" s="95">
-        <f>D19+14</f>
-        <v>45978</v>
+      <c r="D19" s="79">
+        <v>45968</v>
+      </c>
+      <c r="E19" s="79">
+        <v>45970</v>
       </c>
       <c r="F19" s="13"/>
-      <c r="G19" s="3">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
+      <c r="G19" s="3"/>
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
       <c r="J19" s="35"/>
@@ -3321,19 +3333,18 @@
       <c r="BK19" s="35"/>
     </row>
     <row r="20" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="107" t="s">
-        <v>36</v>
+      <c r="A20" s="12"/>
+      <c r="B20" s="91" t="s">
+        <v>65</v>
       </c>
       <c r="C20" s="42">
         <v>0</v>
       </c>
-      <c r="D20" s="95">
-        <v>45978</v>
-      </c>
-      <c r="E20" s="95">
-        <f>D20+2</f>
-        <v>45980</v>
+      <c r="D20" s="79">
+        <v>45970</v>
+      </c>
+      <c r="E20" s="79">
+        <v>45972</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="3"/>
@@ -3394,26 +3405,22 @@
       <c r="BJ20" s="35"/>
       <c r="BK20" s="35"/>
     </row>
-    <row r="21" spans="1:63" s="32" customFormat="1" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="107" t="s">
-        <v>41</v>
+    <row r="21" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="91" t="s">
+        <v>66</v>
       </c>
       <c r="C21" s="42">
         <v>0</v>
       </c>
-      <c r="D21" s="95">
-        <v>45978</v>
-      </c>
-      <c r="E21" s="95">
-        <f>D21+7</f>
-        <v>45985</v>
+      <c r="D21" s="79">
+        <v>45970</v>
+      </c>
+      <c r="E21" s="79">
+        <v>45972</v>
       </c>
       <c r="F21" s="13"/>
-      <c r="G21" s="3">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
+      <c r="G21" s="3"/>
       <c r="H21" s="35"/>
       <c r="I21" s="35"/>
       <c r="J21" s="35"/>
@@ -3430,7 +3437,7 @@
       <c r="U21" s="35"/>
       <c r="V21" s="35"/>
       <c r="W21" s="35"/>
-      <c r="X21" s="38"/>
+      <c r="X21" s="35"/>
       <c r="Y21" s="35"/>
       <c r="Z21" s="35"/>
       <c r="AA21" s="35"/>
@@ -3472,19 +3479,18 @@
       <c r="BK21" s="35"/>
     </row>
     <row r="22" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="41" t="s">
-        <v>37</v>
+      <c r="A22" s="12"/>
+      <c r="B22" s="91" t="s">
+        <v>67</v>
       </c>
       <c r="C22" s="42">
         <v>0</v>
       </c>
-      <c r="D22" s="95">
-        <v>45985</v>
-      </c>
-      <c r="E22" s="95">
-        <f>D22+7</f>
-        <v>45992</v>
+      <c r="D22" s="79">
+        <v>45970</v>
+      </c>
+      <c r="E22" s="79">
+        <v>45972</v>
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="3"/>
@@ -3504,7 +3510,7 @@
       <c r="U22" s="35"/>
       <c r="V22" s="35"/>
       <c r="W22" s="35"/>
-      <c r="X22" s="38"/>
+      <c r="X22" s="35"/>
       <c r="Y22" s="35"/>
       <c r="Z22" s="35"/>
       <c r="AA22" s="35"/>
@@ -3545,20 +3551,19 @@
       <c r="BJ22" s="35"/>
       <c r="BK22" s="35"/>
     </row>
-    <row r="23" spans="1:63" s="32" customFormat="1" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="107" t="s">
-        <v>38</v>
+    <row r="23" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="91" t="s">
+        <v>68</v>
       </c>
       <c r="C23" s="42">
         <v>0</v>
       </c>
-      <c r="D23" s="95">
-        <v>45985</v>
-      </c>
-      <c r="E23" s="95">
-        <f>D23+7</f>
-        <v>45992</v>
+      <c r="D23" s="79">
+        <v>45970</v>
+      </c>
+      <c r="E23" s="79">
+        <v>45972</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="3"/>
@@ -3578,7 +3583,7 @@
       <c r="U23" s="35"/>
       <c r="V23" s="35"/>
       <c r="W23" s="35"/>
-      <c r="X23" s="38"/>
+      <c r="X23" s="35"/>
       <c r="Y23" s="35"/>
       <c r="Z23" s="35"/>
       <c r="AA23" s="35"/>
@@ -3619,20 +3624,20 @@
       <c r="BJ23" s="35"/>
       <c r="BK23" s="35"/>
     </row>
-    <row r="24" spans="1:63" s="32" customFormat="1" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="107" t="s">
-        <v>42</v>
+    <row r="24" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12"/>
+      <c r="B24" s="41" t="s">
+        <v>34</v>
       </c>
       <c r="C24" s="42">
         <v>0</v>
       </c>
-      <c r="D24" s="95">
-        <v>45992</v>
-      </c>
-      <c r="E24" s="95">
-        <f>D24+7</f>
-        <v>45999</v>
+      <c r="D24" s="79">
+        <v>45973</v>
+      </c>
+      <c r="E24" s="79">
+        <f>D24+1</f>
+        <v>45974</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="3"/>
@@ -3652,7 +3657,7 @@
       <c r="U24" s="35"/>
       <c r="V24" s="35"/>
       <c r="W24" s="35"/>
-      <c r="X24" s="38"/>
+      <c r="X24" s="35"/>
       <c r="Y24" s="35"/>
       <c r="Z24" s="35"/>
       <c r="AA24" s="35"/>
@@ -3693,23 +3698,26 @@
       <c r="BJ24" s="35"/>
       <c r="BK24" s="35"/>
     </row>
-    <row r="25" spans="1:63" s="32" customFormat="1" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
-      <c r="B25" s="107" t="s">
-        <v>57</v>
+      <c r="B25" s="41" t="s">
+        <v>35</v>
       </c>
       <c r="C25" s="42">
         <v>0</v>
       </c>
-      <c r="D25" s="95">
-        <v>45999</v>
-      </c>
-      <c r="E25" s="95">
-        <f>D25+7</f>
-        <v>46006</v>
+      <c r="D25" s="79">
+        <f>D24</f>
+        <v>45973</v>
+      </c>
+      <c r="E25" s="79">
+        <v>45974</v>
       </c>
       <c r="F25" s="13"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="3">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
       <c r="H25" s="35"/>
       <c r="I25" s="35"/>
       <c r="J25" s="35"/>
@@ -3722,11 +3730,11 @@
       <c r="Q25" s="35"/>
       <c r="R25" s="35"/>
       <c r="S25" s="35"/>
-      <c r="T25" s="35"/>
-      <c r="U25" s="35"/>
+      <c r="T25" s="38"/>
+      <c r="U25" s="38"/>
       <c r="V25" s="35"/>
       <c r="W25" s="35"/>
-      <c r="X25" s="38"/>
+      <c r="X25" s="35"/>
       <c r="Y25" s="35"/>
       <c r="Z25" s="35"/>
       <c r="AA25" s="35"/>
@@ -3767,25 +3775,25 @@
       <c r="BJ25" s="35"/>
       <c r="BK25" s="35"/>
     </row>
-    <row r="26" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:63" s="32" customFormat="1" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
-      <c r="B26" s="41" t="s">
-        <v>48</v>
+      <c r="B26" s="91" t="s">
+        <v>39</v>
       </c>
       <c r="C26" s="42">
         <v>0</v>
       </c>
-      <c r="D26" s="95">
-        <v>45999</v>
-      </c>
-      <c r="E26" s="95">
-        <f>D26+7</f>
-        <v>46006</v>
+      <c r="D26" s="79">
+        <v>45974</v>
+      </c>
+      <c r="E26" s="79">
+        <f>D26+5</f>
+        <v>45979</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="3">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H26" s="35"/>
       <c r="I26" s="35"/>
@@ -3846,93 +3854,91 @@
     </row>
     <row r="27" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
-      <c r="B27" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="96">
-        <v>46026</v>
-      </c>
-      <c r="E27" s="97">
-        <f>D27+28</f>
-        <v>46054</v>
+      <c r="B27" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="42">
+        <v>0</v>
+      </c>
+      <c r="D27" s="79">
+        <v>45979</v>
+      </c>
+      <c r="E27" s="79">
+        <v>45980</v>
       </c>
       <c r="F27" s="13"/>
-      <c r="G27" s="3">
-        <f t="shared" si="5"/>
-        <v>29</v>
-      </c>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="45"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="45"/>
-      <c r="U27" s="45"/>
-      <c r="V27" s="45"/>
-      <c r="W27" s="45"/>
-      <c r="X27" s="45"/>
-      <c r="Y27" s="45"/>
-      <c r="Z27" s="45"/>
-      <c r="AA27" s="45"/>
-      <c r="AB27" s="45"/>
-      <c r="AC27" s="45"/>
-      <c r="AD27" s="45"/>
-      <c r="AE27" s="45"/>
-      <c r="AF27" s="45"/>
-      <c r="AG27" s="45"/>
-      <c r="AH27" s="45"/>
-      <c r="AI27" s="45"/>
-      <c r="AJ27" s="45"/>
-      <c r="AK27" s="45"/>
-      <c r="AL27" s="45"/>
-      <c r="AM27" s="45"/>
-      <c r="AN27" s="45"/>
-      <c r="AO27" s="45"/>
-      <c r="AP27" s="45"/>
-      <c r="AQ27" s="45"/>
-      <c r="AR27" s="45"/>
-      <c r="AS27" s="45"/>
-      <c r="AT27" s="45"/>
-      <c r="AU27" s="45"/>
-      <c r="AV27" s="45"/>
-      <c r="AW27" s="45"/>
-      <c r="AX27" s="45"/>
-      <c r="AY27" s="45"/>
-      <c r="AZ27" s="45"/>
-      <c r="BA27" s="45"/>
-      <c r="BB27" s="45"/>
-      <c r="BC27" s="45"/>
-      <c r="BD27" s="45"/>
-      <c r="BE27" s="45"/>
-      <c r="BF27" s="45"/>
-      <c r="BG27" s="45"/>
-      <c r="BH27" s="45"/>
-      <c r="BI27" s="45"/>
-      <c r="BJ27" s="45"/>
-      <c r="BK27" s="45"/>
-    </row>
-    <row r="28" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="3"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="35"/>
+      <c r="V27" s="35"/>
+      <c r="W27" s="35"/>
+      <c r="X27" s="35"/>
+      <c r="Y27" s="35"/>
+      <c r="Z27" s="35"/>
+      <c r="AA27" s="35"/>
+      <c r="AB27" s="35"/>
+      <c r="AC27" s="35"/>
+      <c r="AD27" s="35"/>
+      <c r="AE27" s="35"/>
+      <c r="AF27" s="35"/>
+      <c r="AG27" s="35"/>
+      <c r="AH27" s="35"/>
+      <c r="AI27" s="35"/>
+      <c r="AJ27" s="35"/>
+      <c r="AK27" s="35"/>
+      <c r="AL27" s="35"/>
+      <c r="AM27" s="35"/>
+      <c r="AN27" s="35"/>
+      <c r="AO27" s="35"/>
+      <c r="AP27" s="35"/>
+      <c r="AQ27" s="35"/>
+      <c r="AR27" s="35"/>
+      <c r="AS27" s="35"/>
+      <c r="AT27" s="35"/>
+      <c r="AU27" s="35"/>
+      <c r="AV27" s="35"/>
+      <c r="AW27" s="35"/>
+      <c r="AX27" s="35"/>
+      <c r="AY27" s="35"/>
+      <c r="AZ27" s="35"/>
+      <c r="BA27" s="35"/>
+      <c r="BB27" s="35"/>
+      <c r="BC27" s="35"/>
+      <c r="BD27" s="35"/>
+      <c r="BE27" s="35"/>
+      <c r="BF27" s="35"/>
+      <c r="BG27" s="35"/>
+      <c r="BH27" s="35"/>
+      <c r="BI27" s="35"/>
+      <c r="BJ27" s="35"/>
+      <c r="BK27" s="35"/>
+    </row>
+    <row r="28" spans="1:63" s="32" customFormat="1" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
-      <c r="B28" s="109" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="47">
+      <c r="B28" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="42">
         <v>0</v>
       </c>
-      <c r="D28" s="98">
-        <v>46026</v>
-      </c>
-      <c r="E28" s="98">
-        <f>D28+7</f>
-        <v>46033</v>
+      <c r="D28" s="79">
+        <v>45980</v>
+      </c>
+      <c r="E28" s="79">
+        <f t="shared" ref="E28:E33" si="6">D28+7</f>
+        <v>45987</v>
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="3">
@@ -3955,7 +3961,7 @@
       <c r="U28" s="35"/>
       <c r="V28" s="35"/>
       <c r="W28" s="35"/>
-      <c r="X28" s="35"/>
+      <c r="X28" s="38"/>
       <c r="Y28" s="35"/>
       <c r="Z28" s="35"/>
       <c r="AA28" s="35"/>
@@ -3998,24 +4004,21 @@
     </row>
     <row r="29" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
-      <c r="B29" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="47">
+      <c r="B29" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="42">
         <v>0</v>
       </c>
-      <c r="D29" s="98">
-        <v>46033</v>
-      </c>
-      <c r="E29" s="98">
-        <f>D29+7</f>
-        <v>46040</v>
+      <c r="D29" s="79">
+        <v>45980</v>
+      </c>
+      <c r="E29" s="79">
+        <f t="shared" si="6"/>
+        <v>45987</v>
       </c>
       <c r="F29" s="13"/>
-      <c r="G29" s="3">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
+      <c r="G29" s="3"/>
       <c r="H29" s="35"/>
       <c r="I29" s="35"/>
       <c r="J29" s="35"/>
@@ -4032,7 +4035,7 @@
       <c r="U29" s="35"/>
       <c r="V29" s="35"/>
       <c r="W29" s="35"/>
-      <c r="X29" s="35"/>
+      <c r="X29" s="38"/>
       <c r="Y29" s="35"/>
       <c r="Z29" s="35"/>
       <c r="AA29" s="35"/>
@@ -4073,26 +4076,23 @@
       <c r="BJ29" s="35"/>
       <c r="BK29" s="35"/>
     </row>
-    <row r="30" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:63" s="32" customFormat="1" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
-      <c r="B30" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="47">
+      <c r="B30" s="91" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="42">
         <v>0</v>
       </c>
-      <c r="D30" s="98">
-        <v>46040</v>
-      </c>
-      <c r="E30" s="98">
-        <f>D30+7</f>
-        <v>46047</v>
+      <c r="D30" s="79">
+        <v>45980</v>
+      </c>
+      <c r="E30" s="79">
+        <f t="shared" si="6"/>
+        <v>45987</v>
       </c>
       <c r="F30" s="13"/>
-      <c r="G30" s="3">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
+      <c r="G30" s="3"/>
       <c r="H30" s="35"/>
       <c r="I30" s="35"/>
       <c r="J30" s="35"/>
@@ -4109,7 +4109,7 @@
       <c r="U30" s="35"/>
       <c r="V30" s="35"/>
       <c r="W30" s="35"/>
-      <c r="X30" s="35"/>
+      <c r="X30" s="38"/>
       <c r="Y30" s="35"/>
       <c r="Z30" s="35"/>
       <c r="AA30" s="35"/>
@@ -4150,26 +4150,23 @@
       <c r="BJ30" s="35"/>
       <c r="BK30" s="35"/>
     </row>
-    <row r="31" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:63" s="32" customFormat="1" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
-      <c r="B31" s="109" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="47">
+      <c r="B31" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="42">
         <v>0</v>
       </c>
-      <c r="D31" s="98">
-        <v>46047</v>
-      </c>
-      <c r="E31" s="98">
-        <f>D31+3</f>
-        <v>46050</v>
+      <c r="D31" s="79">
+        <v>46017</v>
+      </c>
+      <c r="E31" s="79">
+        <f t="shared" si="6"/>
+        <v>46024</v>
       </c>
       <c r="F31" s="13"/>
-      <c r="G31" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
+      <c r="G31" s="3"/>
       <c r="H31" s="35"/>
       <c r="I31" s="35"/>
       <c r="J31" s="35"/>
@@ -4186,7 +4183,7 @@
       <c r="U31" s="35"/>
       <c r="V31" s="35"/>
       <c r="W31" s="35"/>
-      <c r="X31" s="35"/>
+      <c r="X31" s="38"/>
       <c r="Y31" s="35"/>
       <c r="Z31" s="35"/>
       <c r="AA31" s="35"/>
@@ -4227,20 +4224,20 @@
       <c r="BJ31" s="35"/>
       <c r="BK31" s="35"/>
     </row>
-    <row r="32" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:63" s="32" customFormat="1" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
-      <c r="B32" s="109" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="47">
+      <c r="B32" s="91" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="42">
         <v>0</v>
       </c>
-      <c r="D32" s="98">
-        <v>46050</v>
-      </c>
-      <c r="E32" s="98">
-        <f>D32+4</f>
-        <v>46054</v>
+      <c r="D32" s="79">
+        <v>45999</v>
+      </c>
+      <c r="E32" s="79">
+        <f t="shared" si="6"/>
+        <v>46006</v>
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="3"/>
@@ -4260,7 +4257,7 @@
       <c r="U32" s="35"/>
       <c r="V32" s="35"/>
       <c r="W32" s="35"/>
-      <c r="X32" s="35"/>
+      <c r="X32" s="38"/>
       <c r="Y32" s="35"/>
       <c r="Z32" s="35"/>
       <c r="AA32" s="35"/>
@@ -4303,18 +4300,18 @@
     </row>
     <row r="33" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
-      <c r="B33" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="47">
+      <c r="B33" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="42">
         <v>0</v>
       </c>
-      <c r="D33" s="98">
-        <v>46047</v>
-      </c>
-      <c r="E33" s="98">
-        <f>D33+7</f>
-        <v>46054</v>
+      <c r="D33" s="79">
+        <v>45999</v>
+      </c>
+      <c r="E33" s="79">
+        <f t="shared" si="6"/>
+        <v>46006</v>
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="3">
@@ -4380,93 +4377,93 @@
     </row>
     <row r="34" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
-      <c r="B34" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="99">
+      <c r="B34" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="44"/>
+      <c r="D34" s="80">
+        <v>46026</v>
+      </c>
+      <c r="E34" s="81">
+        <f>D34+28</f>
         <v>46054</v>
-      </c>
-      <c r="E34" s="100">
-        <f>D34+28</f>
-        <v>46082</v>
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="3">
         <f t="shared" si="5"/>
         <v>29</v>
       </c>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="50"/>
-      <c r="L34" s="50"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="50"/>
-      <c r="P34" s="50"/>
-      <c r="Q34" s="50"/>
-      <c r="R34" s="50"/>
-      <c r="S34" s="50"/>
-      <c r="T34" s="50"/>
-      <c r="U34" s="50"/>
-      <c r="V34" s="50"/>
-      <c r="W34" s="50"/>
-      <c r="X34" s="50"/>
-      <c r="Y34" s="50"/>
-      <c r="Z34" s="50"/>
-      <c r="AA34" s="50"/>
-      <c r="AB34" s="50"/>
-      <c r="AC34" s="50"/>
-      <c r="AD34" s="50"/>
-      <c r="AE34" s="50"/>
-      <c r="AF34" s="50"/>
-      <c r="AG34" s="50"/>
-      <c r="AH34" s="50"/>
-      <c r="AI34" s="50"/>
-      <c r="AJ34" s="50"/>
-      <c r="AK34" s="50"/>
-      <c r="AL34" s="50"/>
-      <c r="AM34" s="50"/>
-      <c r="AN34" s="50"/>
-      <c r="AO34" s="50"/>
-      <c r="AP34" s="50"/>
-      <c r="AQ34" s="50"/>
-      <c r="AR34" s="50"/>
-      <c r="AS34" s="50"/>
-      <c r="AT34" s="50"/>
-      <c r="AU34" s="50"/>
-      <c r="AV34" s="50"/>
-      <c r="AW34" s="50"/>
-      <c r="AX34" s="50"/>
-      <c r="AY34" s="50"/>
-      <c r="AZ34" s="50"/>
-      <c r="BA34" s="50"/>
-      <c r="BB34" s="50"/>
-      <c r="BC34" s="50"/>
-      <c r="BD34" s="50"/>
-      <c r="BE34" s="50"/>
-      <c r="BF34" s="50"/>
-      <c r="BG34" s="50"/>
-      <c r="BH34" s="50"/>
-      <c r="BI34" s="50"/>
-      <c r="BJ34" s="50"/>
-      <c r="BK34" s="50"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="45"/>
+      <c r="T34" s="45"/>
+      <c r="U34" s="45"/>
+      <c r="V34" s="45"/>
+      <c r="W34" s="45"/>
+      <c r="X34" s="45"/>
+      <c r="Y34" s="45"/>
+      <c r="Z34" s="45"/>
+      <c r="AA34" s="45"/>
+      <c r="AB34" s="45"/>
+      <c r="AC34" s="45"/>
+      <c r="AD34" s="45"/>
+      <c r="AE34" s="45"/>
+      <c r="AF34" s="45"/>
+      <c r="AG34" s="45"/>
+      <c r="AH34" s="45"/>
+      <c r="AI34" s="45"/>
+      <c r="AJ34" s="45"/>
+      <c r="AK34" s="45"/>
+      <c r="AL34" s="45"/>
+      <c r="AM34" s="45"/>
+      <c r="AN34" s="45"/>
+      <c r="AO34" s="45"/>
+      <c r="AP34" s="45"/>
+      <c r="AQ34" s="45"/>
+      <c r="AR34" s="45"/>
+      <c r="AS34" s="45"/>
+      <c r="AT34" s="45"/>
+      <c r="AU34" s="45"/>
+      <c r="AV34" s="45"/>
+      <c r="AW34" s="45"/>
+      <c r="AX34" s="45"/>
+      <c r="AY34" s="45"/>
+      <c r="AZ34" s="45"/>
+      <c r="BA34" s="45"/>
+      <c r="BB34" s="45"/>
+      <c r="BC34" s="45"/>
+      <c r="BD34" s="45"/>
+      <c r="BE34" s="45"/>
+      <c r="BF34" s="45"/>
+      <c r="BG34" s="45"/>
+      <c r="BH34" s="45"/>
+      <c r="BI34" s="45"/>
+      <c r="BJ34" s="45"/>
+      <c r="BK34" s="45"/>
     </row>
     <row r="35" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
-      <c r="B35" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="52">
+      <c r="B35" s="93" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="47">
         <v>0</v>
       </c>
-      <c r="D35" s="101">
-        <v>46054</v>
-      </c>
-      <c r="E35" s="101">
+      <c r="D35" s="82">
+        <v>46026</v>
+      </c>
+      <c r="E35" s="82">
         <f>D35+7</f>
-        <v>46061</v>
+        <v>46033</v>
       </c>
       <c r="F35" s="13"/>
       <c r="G35" s="3">
@@ -4532,21 +4529,24 @@
     </row>
     <row r="36" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
-      <c r="B36" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="52">
+      <c r="B36" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="47">
         <v>0</v>
       </c>
-      <c r="D36" s="101">
-        <v>46054</v>
-      </c>
-      <c r="E36" s="101">
-        <f>D36+2</f>
-        <v>46056</v>
+      <c r="D36" s="82">
+        <v>46033</v>
+      </c>
+      <c r="E36" s="82">
+        <f>D36+7</f>
+        <v>46040</v>
       </c>
       <c r="F36" s="13"/>
-      <c r="G36" s="3"/>
+      <c r="G36" s="3">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="H36" s="35"/>
       <c r="I36" s="35"/>
       <c r="J36" s="35"/>
@@ -4606,21 +4606,24 @@
     </row>
     <row r="37" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
-      <c r="B37" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="52">
+      <c r="B37" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="47">
         <v>0</v>
       </c>
-      <c r="D37" s="101">
-        <v>46054</v>
-      </c>
-      <c r="E37" s="101">
-        <f>D37+2</f>
-        <v>46056</v>
+      <c r="D37" s="82">
+        <v>46040</v>
+      </c>
+      <c r="E37" s="82">
+        <f>D37+7</f>
+        <v>46047</v>
       </c>
       <c r="F37" s="13"/>
-      <c r="G37" s="3"/>
+      <c r="G37" s="3">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="H37" s="35"/>
       <c r="I37" s="35"/>
       <c r="J37" s="35"/>
@@ -4680,23 +4683,23 @@
     </row>
     <row r="38" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
-      <c r="B38" s="108" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="52">
+      <c r="B38" s="93" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="47">
         <v>0</v>
       </c>
-      <c r="D38" s="101">
-        <v>46061</v>
-      </c>
-      <c r="E38" s="101">
-        <f>D38+4</f>
-        <v>46065</v>
+      <c r="D38" s="82">
+        <v>46047</v>
+      </c>
+      <c r="E38" s="82">
+        <f>D38+3</f>
+        <v>46050</v>
       </c>
       <c r="F38" s="13"/>
       <c r="G38" s="3">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H38" s="35"/>
       <c r="I38" s="35"/>
@@ -4757,24 +4760,21 @@
     </row>
     <row r="39" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11"/>
-      <c r="B39" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="52">
+      <c r="B39" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="47">
         <v>0</v>
       </c>
-      <c r="D39" s="101">
-        <v>46061</v>
-      </c>
-      <c r="E39" s="101">
+      <c r="D39" s="82">
+        <v>46050</v>
+      </c>
+      <c r="E39" s="82">
         <f>D39+4</f>
-        <v>46065</v>
+        <v>46054</v>
       </c>
       <c r="F39" s="13"/>
-      <c r="G39" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
+      <c r="G39" s="3"/>
       <c r="H39" s="35"/>
       <c r="I39" s="35"/>
       <c r="J39" s="35"/>
@@ -4832,20 +4832,20 @@
       <c r="BJ39" s="35"/>
       <c r="BK39" s="35"/>
     </row>
-    <row r="40" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11"/>
-      <c r="B40" s="108" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="52">
+      <c r="B40" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="47">
         <v>0</v>
       </c>
-      <c r="D40" s="101">
-        <v>46065</v>
-      </c>
-      <c r="E40" s="101">
+      <c r="D40" s="82">
+        <v>46047</v>
+      </c>
+      <c r="E40" s="82">
         <f>D40+7</f>
-        <v>46072</v>
+        <v>46054</v>
       </c>
       <c r="F40" s="13"/>
       <c r="G40" s="3">
@@ -4909,94 +4909,95 @@
       <c r="BJ40" s="35"/>
       <c r="BK40" s="35"/>
     </row>
-    <row r="41" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11"/>
-      <c r="B41" s="108" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="52">
-        <v>0</v>
-      </c>
-      <c r="D41" s="101">
-        <v>46072</v>
-      </c>
-      <c r="E41" s="101">
-        <f>D41+7</f>
-        <v>46079</v>
+      <c r="B41" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="49"/>
+      <c r="D41" s="83">
+        <v>46054</v>
+      </c>
+      <c r="E41" s="84">
+        <f>D41+28</f>
+        <v>46082</v>
       </c>
       <c r="F41" s="13"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35"/>
-      <c r="L41" s="35"/>
-      <c r="M41" s="35"/>
-      <c r="N41" s="35"/>
-      <c r="O41" s="35"/>
-      <c r="P41" s="35"/>
-      <c r="Q41" s="35"/>
-      <c r="R41" s="35"/>
-      <c r="S41" s="35"/>
-      <c r="T41" s="35"/>
-      <c r="U41" s="35"/>
-      <c r="V41" s="35"/>
-      <c r="W41" s="35"/>
-      <c r="X41" s="35"/>
-      <c r="Y41" s="35"/>
-      <c r="Z41" s="35"/>
-      <c r="AA41" s="35"/>
-      <c r="AB41" s="35"/>
-      <c r="AC41" s="35"/>
-      <c r="AD41" s="35"/>
-      <c r="AE41" s="35"/>
-      <c r="AF41" s="35"/>
-      <c r="AG41" s="35"/>
-      <c r="AH41" s="35"/>
-      <c r="AI41" s="35"/>
-      <c r="AJ41" s="35"/>
-      <c r="AK41" s="35"/>
-      <c r="AL41" s="35"/>
-      <c r="AM41" s="35"/>
-      <c r="AN41" s="35"/>
-      <c r="AO41" s="35"/>
-      <c r="AP41" s="35"/>
-      <c r="AQ41" s="35"/>
-      <c r="AR41" s="35"/>
-      <c r="AS41" s="35"/>
-      <c r="AT41" s="35"/>
-      <c r="AU41" s="35"/>
-      <c r="AV41" s="35"/>
-      <c r="AW41" s="35"/>
-      <c r="AX41" s="35"/>
-      <c r="AY41" s="35"/>
-      <c r="AZ41" s="35"/>
-      <c r="BA41" s="35"/>
-      <c r="BB41" s="35"/>
-      <c r="BC41" s="35"/>
-      <c r="BD41" s="35"/>
-      <c r="BE41" s="35"/>
-      <c r="BF41" s="35"/>
-      <c r="BG41" s="35"/>
-      <c r="BH41" s="35"/>
-      <c r="BI41" s="35"/>
-      <c r="BJ41" s="35"/>
-      <c r="BK41" s="35"/>
+      <c r="G41" s="3">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="50"/>
+      <c r="L41" s="50"/>
+      <c r="M41" s="50"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="50"/>
+      <c r="P41" s="50"/>
+      <c r="Q41" s="50"/>
+      <c r="R41" s="50"/>
+      <c r="S41" s="50"/>
+      <c r="T41" s="50"/>
+      <c r="U41" s="50"/>
+      <c r="V41" s="50"/>
+      <c r="W41" s="50"/>
+      <c r="X41" s="50"/>
+      <c r="Y41" s="50"/>
+      <c r="Z41" s="50"/>
+      <c r="AA41" s="50"/>
+      <c r="AB41" s="50"/>
+      <c r="AC41" s="50"/>
+      <c r="AD41" s="50"/>
+      <c r="AE41" s="50"/>
+      <c r="AF41" s="50"/>
+      <c r="AG41" s="50"/>
+      <c r="AH41" s="50"/>
+      <c r="AI41" s="50"/>
+      <c r="AJ41" s="50"/>
+      <c r="AK41" s="50"/>
+      <c r="AL41" s="50"/>
+      <c r="AM41" s="50"/>
+      <c r="AN41" s="50"/>
+      <c r="AO41" s="50"/>
+      <c r="AP41" s="50"/>
+      <c r="AQ41" s="50"/>
+      <c r="AR41" s="50"/>
+      <c r="AS41" s="50"/>
+      <c r="AT41" s="50"/>
+      <c r="AU41" s="50"/>
+      <c r="AV41" s="50"/>
+      <c r="AW41" s="50"/>
+      <c r="AX41" s="50"/>
+      <c r="AY41" s="50"/>
+      <c r="AZ41" s="50"/>
+      <c r="BA41" s="50"/>
+      <c r="BB41" s="50"/>
+      <c r="BC41" s="50"/>
+      <c r="BD41" s="50"/>
+      <c r="BE41" s="50"/>
+      <c r="BF41" s="50"/>
+      <c r="BG41" s="50"/>
+      <c r="BH41" s="50"/>
+      <c r="BI41" s="50"/>
+      <c r="BJ41" s="50"/>
+      <c r="BK41" s="50"/>
     </row>
     <row r="42" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11"/>
       <c r="B42" s="51" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C42" s="52">
         <v>0</v>
       </c>
-      <c r="D42" s="101">
-        <v>46075</v>
-      </c>
-      <c r="E42" s="101">
+      <c r="D42" s="85">
+        <v>46054</v>
+      </c>
+      <c r="E42" s="85">
         <f>D42+7</f>
-        <v>46082</v>
+        <v>46061</v>
       </c>
       <c r="F42" s="13"/>
       <c r="G42" s="3">
@@ -5062,92 +5063,92 @@
     </row>
     <row r="43" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11"/>
-      <c r="B43" s="115" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="110"/>
-      <c r="D43" s="111">
-        <v>46083</v>
-      </c>
-      <c r="E43" s="111">
-        <v>46147</v>
+      <c r="B43" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="52">
+        <v>0</v>
+      </c>
+      <c r="D43" s="85">
+        <v>46054</v>
+      </c>
+      <c r="E43" s="85">
+        <f>D43+2</f>
+        <v>46056</v>
       </c>
       <c r="F43" s="13"/>
-      <c r="G43" s="3">
-        <f t="shared" si="5"/>
-        <v>65</v>
-      </c>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="31"/>
-      <c r="O43" s="31"/>
-      <c r="P43" s="31"/>
-      <c r="Q43" s="31"/>
-      <c r="R43" s="31"/>
-      <c r="S43" s="31"/>
-      <c r="T43" s="31"/>
-      <c r="U43" s="31"/>
-      <c r="V43" s="31"/>
-      <c r="W43" s="31"/>
-      <c r="X43" s="31"/>
-      <c r="Y43" s="31"/>
-      <c r="Z43" s="31"/>
-      <c r="AA43" s="31"/>
-      <c r="AB43" s="31"/>
-      <c r="AC43" s="31"/>
-      <c r="AD43" s="31"/>
-      <c r="AE43" s="31"/>
-      <c r="AF43" s="31"/>
-      <c r="AG43" s="31"/>
-      <c r="AH43" s="31"/>
-      <c r="AI43" s="31"/>
-      <c r="AJ43" s="31"/>
-      <c r="AK43" s="31"/>
-      <c r="AL43" s="31"/>
-      <c r="AM43" s="31"/>
-      <c r="AN43" s="31"/>
-      <c r="AO43" s="31"/>
-      <c r="AP43" s="31"/>
-      <c r="AQ43" s="31"/>
-      <c r="AR43" s="31"/>
-      <c r="AS43" s="31"/>
-      <c r="AT43" s="31"/>
-      <c r="AU43" s="31"/>
-      <c r="AV43" s="31"/>
-      <c r="AW43" s="31"/>
-      <c r="AX43" s="31"/>
-      <c r="AY43" s="31"/>
-      <c r="AZ43" s="31"/>
-      <c r="BA43" s="31"/>
-      <c r="BB43" s="31"/>
-      <c r="BC43" s="31"/>
-      <c r="BD43" s="31"/>
-      <c r="BE43" s="31"/>
-      <c r="BF43" s="31"/>
-      <c r="BG43" s="31"/>
-      <c r="BH43" s="31"/>
-      <c r="BI43" s="31"/>
-      <c r="BJ43" s="31"/>
-      <c r="BK43" s="31"/>
-    </row>
-    <row r="44" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G43" s="3"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="35"/>
+      <c r="S43" s="35"/>
+      <c r="T43" s="35"/>
+      <c r="U43" s="35"/>
+      <c r="V43" s="35"/>
+      <c r="W43" s="35"/>
+      <c r="X43" s="35"/>
+      <c r="Y43" s="35"/>
+      <c r="Z43" s="35"/>
+      <c r="AA43" s="35"/>
+      <c r="AB43" s="35"/>
+      <c r="AC43" s="35"/>
+      <c r="AD43" s="35"/>
+      <c r="AE43" s="35"/>
+      <c r="AF43" s="35"/>
+      <c r="AG43" s="35"/>
+      <c r="AH43" s="35"/>
+      <c r="AI43" s="35"/>
+      <c r="AJ43" s="35"/>
+      <c r="AK43" s="35"/>
+      <c r="AL43" s="35"/>
+      <c r="AM43" s="35"/>
+      <c r="AN43" s="35"/>
+      <c r="AO43" s="35"/>
+      <c r="AP43" s="35"/>
+      <c r="AQ43" s="35"/>
+      <c r="AR43" s="35"/>
+      <c r="AS43" s="35"/>
+      <c r="AT43" s="35"/>
+      <c r="AU43" s="35"/>
+      <c r="AV43" s="35"/>
+      <c r="AW43" s="35"/>
+      <c r="AX43" s="35"/>
+      <c r="AY43" s="35"/>
+      <c r="AZ43" s="35"/>
+      <c r="BA43" s="35"/>
+      <c r="BB43" s="35"/>
+      <c r="BC43" s="35"/>
+      <c r="BD43" s="35"/>
+      <c r="BE43" s="35"/>
+      <c r="BF43" s="35"/>
+      <c r="BG43" s="35"/>
+      <c r="BH43" s="35"/>
+      <c r="BI43" s="35"/>
+      <c r="BJ43" s="35"/>
+      <c r="BK43" s="35"/>
+    </row>
+    <row r="44" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11"/>
-      <c r="B44" s="112" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="113">
+      <c r="B44" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="52">
         <v>0</v>
       </c>
-      <c r="D44" s="114">
-        <v>46083</v>
-      </c>
-      <c r="E44" s="114">
-        <f>D44+14</f>
-        <v>46097</v>
+      <c r="D44" s="85">
+        <v>46054</v>
+      </c>
+      <c r="E44" s="85">
+        <f>D44+2</f>
+        <v>46056</v>
       </c>
       <c r="F44" s="13"/>
       <c r="G44" s="3"/>
@@ -5208,23 +5209,26 @@
       <c r="BJ44" s="35"/>
       <c r="BK44" s="35"/>
     </row>
-    <row r="45" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11"/>
-      <c r="B45" s="112" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="113">
+      <c r="B45" s="92" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="52">
         <v>0</v>
       </c>
-      <c r="D45" s="114">
-        <v>46098</v>
-      </c>
-      <c r="E45" s="114">
-        <f>D45+42</f>
-        <v>46140</v>
+      <c r="D45" s="85">
+        <v>46061</v>
+      </c>
+      <c r="E45" s="85">
+        <f>D45+4</f>
+        <v>46065</v>
       </c>
       <c r="F45" s="13"/>
-      <c r="G45" s="3"/>
+      <c r="G45" s="3">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
       <c r="H45" s="35"/>
       <c r="I45" s="35"/>
       <c r="J45" s="35"/>
@@ -5282,23 +5286,26 @@
       <c r="BJ45" s="35"/>
       <c r="BK45" s="35"/>
     </row>
-    <row r="46" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11"/>
-      <c r="B46" s="112" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" s="113">
+      <c r="B46" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="52">
         <v>0</v>
       </c>
-      <c r="D46" s="114">
-        <v>46083</v>
-      </c>
-      <c r="E46" s="114">
-        <f>D46+64</f>
-        <v>46147</v>
+      <c r="D46" s="85">
+        <v>46061</v>
+      </c>
+      <c r="E46" s="85">
+        <f>D46+4</f>
+        <v>46065</v>
       </c>
       <c r="F46" s="13"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
       <c r="H46" s="35"/>
       <c r="I46" s="35"/>
       <c r="J46" s="35"/>
@@ -5358,12 +5365,24 @@
     </row>
     <row r="47" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11"/>
-      <c r="B47" s="112"/>
-      <c r="C47" s="113"/>
-      <c r="D47" s="114"/>
-      <c r="E47" s="114"/>
+      <c r="B47" s="92" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="52">
+        <v>0</v>
+      </c>
+      <c r="D47" s="85">
+        <v>46065</v>
+      </c>
+      <c r="E47" s="85">
+        <f>D47+7</f>
+        <v>46072</v>
+      </c>
       <c r="F47" s="13"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="H47" s="35"/>
       <c r="I47" s="35"/>
       <c r="J47" s="35"/>
@@ -5421,84 +5440,605 @@
       <c r="BJ47" s="35"/>
       <c r="BK47" s="35"/>
     </row>
-    <row r="48" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="12"/>
-      <c r="B48" s="53" t="s">
+    <row r="48" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="11"/>
+      <c r="B48" s="92" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="52">
+        <v>0</v>
+      </c>
+      <c r="D48" s="85">
+        <v>46072</v>
+      </c>
+      <c r="E48" s="85">
+        <f>D48+7</f>
+        <v>46079</v>
+      </c>
+      <c r="F48" s="13"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
+      <c r="M48" s="35"/>
+      <c r="N48" s="35"/>
+      <c r="O48" s="35"/>
+      <c r="P48" s="35"/>
+      <c r="Q48" s="35"/>
+      <c r="R48" s="35"/>
+      <c r="S48" s="35"/>
+      <c r="T48" s="35"/>
+      <c r="U48" s="35"/>
+      <c r="V48" s="35"/>
+      <c r="W48" s="35"/>
+      <c r="X48" s="35"/>
+      <c r="Y48" s="35"/>
+      <c r="Z48" s="35"/>
+      <c r="AA48" s="35"/>
+      <c r="AB48" s="35"/>
+      <c r="AC48" s="35"/>
+      <c r="AD48" s="35"/>
+      <c r="AE48" s="35"/>
+      <c r="AF48" s="35"/>
+      <c r="AG48" s="35"/>
+      <c r="AH48" s="35"/>
+      <c r="AI48" s="35"/>
+      <c r="AJ48" s="35"/>
+      <c r="AK48" s="35"/>
+      <c r="AL48" s="35"/>
+      <c r="AM48" s="35"/>
+      <c r="AN48" s="35"/>
+      <c r="AO48" s="35"/>
+      <c r="AP48" s="35"/>
+      <c r="AQ48" s="35"/>
+      <c r="AR48" s="35"/>
+      <c r="AS48" s="35"/>
+      <c r="AT48" s="35"/>
+      <c r="AU48" s="35"/>
+      <c r="AV48" s="35"/>
+      <c r="AW48" s="35"/>
+      <c r="AX48" s="35"/>
+      <c r="AY48" s="35"/>
+      <c r="AZ48" s="35"/>
+      <c r="BA48" s="35"/>
+      <c r="BB48" s="35"/>
+      <c r="BC48" s="35"/>
+      <c r="BD48" s="35"/>
+      <c r="BE48" s="35"/>
+      <c r="BF48" s="35"/>
+      <c r="BG48" s="35"/>
+      <c r="BH48" s="35"/>
+      <c r="BI48" s="35"/>
+      <c r="BJ48" s="35"/>
+      <c r="BK48" s="35"/>
+    </row>
+    <row r="49" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="11"/>
+      <c r="B49" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="52">
+        <v>0</v>
+      </c>
+      <c r="D49" s="85">
+        <v>46075</v>
+      </c>
+      <c r="E49" s="85">
+        <f>D49+7</f>
+        <v>46082</v>
+      </c>
+      <c r="F49" s="13"/>
+      <c r="G49" s="3">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="35"/>
+      <c r="N49" s="35"/>
+      <c r="O49" s="35"/>
+      <c r="P49" s="35"/>
+      <c r="Q49" s="35"/>
+      <c r="R49" s="35"/>
+      <c r="S49" s="35"/>
+      <c r="T49" s="35"/>
+      <c r="U49" s="35"/>
+      <c r="V49" s="35"/>
+      <c r="W49" s="35"/>
+      <c r="X49" s="35"/>
+      <c r="Y49" s="35"/>
+      <c r="Z49" s="35"/>
+      <c r="AA49" s="35"/>
+      <c r="AB49" s="35"/>
+      <c r="AC49" s="35"/>
+      <c r="AD49" s="35"/>
+      <c r="AE49" s="35"/>
+      <c r="AF49" s="35"/>
+      <c r="AG49" s="35"/>
+      <c r="AH49" s="35"/>
+      <c r="AI49" s="35"/>
+      <c r="AJ49" s="35"/>
+      <c r="AK49" s="35"/>
+      <c r="AL49" s="35"/>
+      <c r="AM49" s="35"/>
+      <c r="AN49" s="35"/>
+      <c r="AO49" s="35"/>
+      <c r="AP49" s="35"/>
+      <c r="AQ49" s="35"/>
+      <c r="AR49" s="35"/>
+      <c r="AS49" s="35"/>
+      <c r="AT49" s="35"/>
+      <c r="AU49" s="35"/>
+      <c r="AV49" s="35"/>
+      <c r="AW49" s="35"/>
+      <c r="AX49" s="35"/>
+      <c r="AY49" s="35"/>
+      <c r="AZ49" s="35"/>
+      <c r="BA49" s="35"/>
+      <c r="BB49" s="35"/>
+      <c r="BC49" s="35"/>
+      <c r="BD49" s="35"/>
+      <c r="BE49" s="35"/>
+      <c r="BF49" s="35"/>
+      <c r="BG49" s="35"/>
+      <c r="BH49" s="35"/>
+      <c r="BI49" s="35"/>
+      <c r="BJ49" s="35"/>
+      <c r="BK49" s="35"/>
+    </row>
+    <row r="50" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="11"/>
+      <c r="B50" s="99" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="94"/>
+      <c r="D50" s="95">
+        <v>46083</v>
+      </c>
+      <c r="E50" s="95">
+        <v>46147</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="3">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="31"/>
+      <c r="K50" s="31"/>
+      <c r="L50" s="31"/>
+      <c r="M50" s="31"/>
+      <c r="N50" s="31"/>
+      <c r="O50" s="31"/>
+      <c r="P50" s="31"/>
+      <c r="Q50" s="31"/>
+      <c r="R50" s="31"/>
+      <c r="S50" s="31"/>
+      <c r="T50" s="31"/>
+      <c r="U50" s="31"/>
+      <c r="V50" s="31"/>
+      <c r="W50" s="31"/>
+      <c r="X50" s="31"/>
+      <c r="Y50" s="31"/>
+      <c r="Z50" s="31"/>
+      <c r="AA50" s="31"/>
+      <c r="AB50" s="31"/>
+      <c r="AC50" s="31"/>
+      <c r="AD50" s="31"/>
+      <c r="AE50" s="31"/>
+      <c r="AF50" s="31"/>
+      <c r="AG50" s="31"/>
+      <c r="AH50" s="31"/>
+      <c r="AI50" s="31"/>
+      <c r="AJ50" s="31"/>
+      <c r="AK50" s="31"/>
+      <c r="AL50" s="31"/>
+      <c r="AM50" s="31"/>
+      <c r="AN50" s="31"/>
+      <c r="AO50" s="31"/>
+      <c r="AP50" s="31"/>
+      <c r="AQ50" s="31"/>
+      <c r="AR50" s="31"/>
+      <c r="AS50" s="31"/>
+      <c r="AT50" s="31"/>
+      <c r="AU50" s="31"/>
+      <c r="AV50" s="31"/>
+      <c r="AW50" s="31"/>
+      <c r="AX50" s="31"/>
+      <c r="AY50" s="31"/>
+      <c r="AZ50" s="31"/>
+      <c r="BA50" s="31"/>
+      <c r="BB50" s="31"/>
+      <c r="BC50" s="31"/>
+      <c r="BD50" s="31"/>
+      <c r="BE50" s="31"/>
+      <c r="BF50" s="31"/>
+      <c r="BG50" s="31"/>
+      <c r="BH50" s="31"/>
+      <c r="BI50" s="31"/>
+      <c r="BJ50" s="31"/>
+      <c r="BK50" s="31"/>
+    </row>
+    <row r="51" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="11"/>
+      <c r="B51" s="96" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="97">
+        <v>0</v>
+      </c>
+      <c r="D51" s="98">
+        <v>46083</v>
+      </c>
+      <c r="E51" s="98">
+        <f>D51+14</f>
+        <v>46097</v>
+      </c>
+      <c r="F51" s="13"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
+      <c r="L51" s="35"/>
+      <c r="M51" s="35"/>
+      <c r="N51" s="35"/>
+      <c r="O51" s="35"/>
+      <c r="P51" s="35"/>
+      <c r="Q51" s="35"/>
+      <c r="R51" s="35"/>
+      <c r="S51" s="35"/>
+      <c r="T51" s="35"/>
+      <c r="U51" s="35"/>
+      <c r="V51" s="35"/>
+      <c r="W51" s="35"/>
+      <c r="X51" s="35"/>
+      <c r="Y51" s="35"/>
+      <c r="Z51" s="35"/>
+      <c r="AA51" s="35"/>
+      <c r="AB51" s="35"/>
+      <c r="AC51" s="35"/>
+      <c r="AD51" s="35"/>
+      <c r="AE51" s="35"/>
+      <c r="AF51" s="35"/>
+      <c r="AG51" s="35"/>
+      <c r="AH51" s="35"/>
+      <c r="AI51" s="35"/>
+      <c r="AJ51" s="35"/>
+      <c r="AK51" s="35"/>
+      <c r="AL51" s="35"/>
+      <c r="AM51" s="35"/>
+      <c r="AN51" s="35"/>
+      <c r="AO51" s="35"/>
+      <c r="AP51" s="35"/>
+      <c r="AQ51" s="35"/>
+      <c r="AR51" s="35"/>
+      <c r="AS51" s="35"/>
+      <c r="AT51" s="35"/>
+      <c r="AU51" s="35"/>
+      <c r="AV51" s="35"/>
+      <c r="AW51" s="35"/>
+      <c r="AX51" s="35"/>
+      <c r="AY51" s="35"/>
+      <c r="AZ51" s="35"/>
+      <c r="BA51" s="35"/>
+      <c r="BB51" s="35"/>
+      <c r="BC51" s="35"/>
+      <c r="BD51" s="35"/>
+      <c r="BE51" s="35"/>
+      <c r="BF51" s="35"/>
+      <c r="BG51" s="35"/>
+      <c r="BH51" s="35"/>
+      <c r="BI51" s="35"/>
+      <c r="BJ51" s="35"/>
+      <c r="BK51" s="35"/>
+    </row>
+    <row r="52" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="11"/>
+      <c r="B52" s="96" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="97">
+        <v>0</v>
+      </c>
+      <c r="D52" s="98">
+        <v>46098</v>
+      </c>
+      <c r="E52" s="98">
+        <f>D52+42</f>
+        <v>46140</v>
+      </c>
+      <c r="F52" s="13"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="35"/>
+      <c r="N52" s="35"/>
+      <c r="O52" s="35"/>
+      <c r="P52" s="35"/>
+      <c r="Q52" s="35"/>
+      <c r="R52" s="35"/>
+      <c r="S52" s="35"/>
+      <c r="T52" s="35"/>
+      <c r="U52" s="35"/>
+      <c r="V52" s="35"/>
+      <c r="W52" s="35"/>
+      <c r="X52" s="35"/>
+      <c r="Y52" s="35"/>
+      <c r="Z52" s="35"/>
+      <c r="AA52" s="35"/>
+      <c r="AB52" s="35"/>
+      <c r="AC52" s="35"/>
+      <c r="AD52" s="35"/>
+      <c r="AE52" s="35"/>
+      <c r="AF52" s="35"/>
+      <c r="AG52" s="35"/>
+      <c r="AH52" s="35"/>
+      <c r="AI52" s="35"/>
+      <c r="AJ52" s="35"/>
+      <c r="AK52" s="35"/>
+      <c r="AL52" s="35"/>
+      <c r="AM52" s="35"/>
+      <c r="AN52" s="35"/>
+      <c r="AO52" s="35"/>
+      <c r="AP52" s="35"/>
+      <c r="AQ52" s="35"/>
+      <c r="AR52" s="35"/>
+      <c r="AS52" s="35"/>
+      <c r="AT52" s="35"/>
+      <c r="AU52" s="35"/>
+      <c r="AV52" s="35"/>
+      <c r="AW52" s="35"/>
+      <c r="AX52" s="35"/>
+      <c r="AY52" s="35"/>
+      <c r="AZ52" s="35"/>
+      <c r="BA52" s="35"/>
+      <c r="BB52" s="35"/>
+      <c r="BC52" s="35"/>
+      <c r="BD52" s="35"/>
+      <c r="BE52" s="35"/>
+      <c r="BF52" s="35"/>
+      <c r="BG52" s="35"/>
+      <c r="BH52" s="35"/>
+      <c r="BI52" s="35"/>
+      <c r="BJ52" s="35"/>
+      <c r="BK52" s="35"/>
+    </row>
+    <row r="53" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="11"/>
+      <c r="B53" s="96" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="97">
+        <v>0</v>
+      </c>
+      <c r="D53" s="98">
+        <v>46083</v>
+      </c>
+      <c r="E53" s="98">
+        <f>D53+64</f>
+        <v>46147</v>
+      </c>
+      <c r="F53" s="13"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="35"/>
+      <c r="L53" s="35"/>
+      <c r="M53" s="35"/>
+      <c r="N53" s="35"/>
+      <c r="O53" s="35"/>
+      <c r="P53" s="35"/>
+      <c r="Q53" s="35"/>
+      <c r="R53" s="35"/>
+      <c r="S53" s="35"/>
+      <c r="T53" s="35"/>
+      <c r="U53" s="35"/>
+      <c r="V53" s="35"/>
+      <c r="W53" s="35"/>
+      <c r="X53" s="35"/>
+      <c r="Y53" s="35"/>
+      <c r="Z53" s="35"/>
+      <c r="AA53" s="35"/>
+      <c r="AB53" s="35"/>
+      <c r="AC53" s="35"/>
+      <c r="AD53" s="35"/>
+      <c r="AE53" s="35"/>
+      <c r="AF53" s="35"/>
+      <c r="AG53" s="35"/>
+      <c r="AH53" s="35"/>
+      <c r="AI53" s="35"/>
+      <c r="AJ53" s="35"/>
+      <c r="AK53" s="35"/>
+      <c r="AL53" s="35"/>
+      <c r="AM53" s="35"/>
+      <c r="AN53" s="35"/>
+      <c r="AO53" s="35"/>
+      <c r="AP53" s="35"/>
+      <c r="AQ53" s="35"/>
+      <c r="AR53" s="35"/>
+      <c r="AS53" s="35"/>
+      <c r="AT53" s="35"/>
+      <c r="AU53" s="35"/>
+      <c r="AV53" s="35"/>
+      <c r="AW53" s="35"/>
+      <c r="AX53" s="35"/>
+      <c r="AY53" s="35"/>
+      <c r="AZ53" s="35"/>
+      <c r="BA53" s="35"/>
+      <c r="BB53" s="35"/>
+      <c r="BC53" s="35"/>
+      <c r="BD53" s="35"/>
+      <c r="BE53" s="35"/>
+      <c r="BF53" s="35"/>
+      <c r="BG53" s="35"/>
+      <c r="BH53" s="35"/>
+      <c r="BI53" s="35"/>
+      <c r="BJ53" s="35"/>
+      <c r="BK53" s="35"/>
+    </row>
+    <row r="54" spans="1:63" s="32" customFormat="1" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="11"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="97"/>
+      <c r="D54" s="98"/>
+      <c r="E54" s="98"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="35"/>
+      <c r="M54" s="35"/>
+      <c r="N54" s="35"/>
+      <c r="O54" s="35"/>
+      <c r="P54" s="35"/>
+      <c r="Q54" s="35"/>
+      <c r="R54" s="35"/>
+      <c r="S54" s="35"/>
+      <c r="T54" s="35"/>
+      <c r="U54" s="35"/>
+      <c r="V54" s="35"/>
+      <c r="W54" s="35"/>
+      <c r="X54" s="35"/>
+      <c r="Y54" s="35"/>
+      <c r="Z54" s="35"/>
+      <c r="AA54" s="35"/>
+      <c r="AB54" s="35"/>
+      <c r="AC54" s="35"/>
+      <c r="AD54" s="35"/>
+      <c r="AE54" s="35"/>
+      <c r="AF54" s="35"/>
+      <c r="AG54" s="35"/>
+      <c r="AH54" s="35"/>
+      <c r="AI54" s="35"/>
+      <c r="AJ54" s="35"/>
+      <c r="AK54" s="35"/>
+      <c r="AL54" s="35"/>
+      <c r="AM54" s="35"/>
+      <c r="AN54" s="35"/>
+      <c r="AO54" s="35"/>
+      <c r="AP54" s="35"/>
+      <c r="AQ54" s="35"/>
+      <c r="AR54" s="35"/>
+      <c r="AS54" s="35"/>
+      <c r="AT54" s="35"/>
+      <c r="AU54" s="35"/>
+      <c r="AV54" s="35"/>
+      <c r="AW54" s="35"/>
+      <c r="AX54" s="35"/>
+      <c r="AY54" s="35"/>
+      <c r="AZ54" s="35"/>
+      <c r="BA54" s="35"/>
+      <c r="BB54" s="35"/>
+      <c r="BC54" s="35"/>
+      <c r="BD54" s="35"/>
+      <c r="BE54" s="35"/>
+      <c r="BF54" s="35"/>
+      <c r="BG54" s="35"/>
+      <c r="BH54" s="35"/>
+      <c r="BI54" s="35"/>
+      <c r="BJ54" s="35"/>
+      <c r="BK54" s="35"/>
+    </row>
+    <row r="55" spans="1:63" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="12"/>
+      <c r="B55" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="54"/>
-      <c r="D48" s="102"/>
-      <c r="E48" s="103"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="4" t="str">
+      <c r="C55" s="54"/>
+      <c r="D55" s="86"/>
+      <c r="E55" s="87"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="4" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="55"/>
-      <c r="L48" s="55"/>
-      <c r="M48" s="55"/>
-      <c r="N48" s="55"/>
-      <c r="O48" s="55"/>
-      <c r="P48" s="55"/>
-      <c r="Q48" s="55"/>
-      <c r="R48" s="55"/>
-      <c r="S48" s="55"/>
-      <c r="T48" s="55"/>
-      <c r="U48" s="55"/>
-      <c r="V48" s="55"/>
-      <c r="W48" s="55"/>
-      <c r="X48" s="55"/>
-      <c r="Y48" s="55"/>
-      <c r="Z48" s="55"/>
-      <c r="AA48" s="55"/>
-      <c r="AB48" s="55"/>
-      <c r="AC48" s="55"/>
-      <c r="AD48" s="55"/>
-      <c r="AE48" s="55"/>
-      <c r="AF48" s="55"/>
-      <c r="AG48" s="55"/>
-      <c r="AH48" s="55"/>
-      <c r="AI48" s="55"/>
-      <c r="AJ48" s="55"/>
-      <c r="AK48" s="55"/>
-      <c r="AL48" s="55"/>
-      <c r="AM48" s="55"/>
-      <c r="AN48" s="55"/>
-      <c r="AO48" s="55"/>
-      <c r="AP48" s="55"/>
-      <c r="AQ48" s="55"/>
-      <c r="AR48" s="55"/>
-      <c r="AS48" s="55"/>
-      <c r="AT48" s="55"/>
-      <c r="AU48" s="55"/>
-      <c r="AV48" s="55"/>
-      <c r="AW48" s="55"/>
-      <c r="AX48" s="55"/>
-      <c r="AY48" s="55"/>
-      <c r="AZ48" s="55"/>
-      <c r="BA48" s="55"/>
-      <c r="BB48" s="55"/>
-      <c r="BC48" s="55"/>
-      <c r="BD48" s="55"/>
-      <c r="BE48" s="55"/>
-      <c r="BF48" s="55"/>
-      <c r="BG48" s="55"/>
-      <c r="BH48" s="55"/>
-      <c r="BI48" s="55"/>
-      <c r="BJ48" s="55"/>
-      <c r="BK48" s="55"/>
-    </row>
-    <row r="49" spans="5:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="5:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E50" s="106"/>
+      <c r="H55" s="55"/>
+      <c r="I55" s="55"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="55"/>
+      <c r="L55" s="55"/>
+      <c r="M55" s="55"/>
+      <c r="N55" s="55"/>
+      <c r="O55" s="55"/>
+      <c r="P55" s="55"/>
+      <c r="Q55" s="55"/>
+      <c r="R55" s="55"/>
+      <c r="S55" s="55"/>
+      <c r="T55" s="55"/>
+      <c r="U55" s="55"/>
+      <c r="V55" s="55"/>
+      <c r="W55" s="55"/>
+      <c r="X55" s="55"/>
+      <c r="Y55" s="55"/>
+      <c r="Z55" s="55"/>
+      <c r="AA55" s="55"/>
+      <c r="AB55" s="55"/>
+      <c r="AC55" s="55"/>
+      <c r="AD55" s="55"/>
+      <c r="AE55" s="55"/>
+      <c r="AF55" s="55"/>
+      <c r="AG55" s="55"/>
+      <c r="AH55" s="55"/>
+      <c r="AI55" s="55"/>
+      <c r="AJ55" s="55"/>
+      <c r="AK55" s="55"/>
+      <c r="AL55" s="55"/>
+      <c r="AM55" s="55"/>
+      <c r="AN55" s="55"/>
+      <c r="AO55" s="55"/>
+      <c r="AP55" s="55"/>
+      <c r="AQ55" s="55"/>
+      <c r="AR55" s="55"/>
+      <c r="AS55" s="55"/>
+      <c r="AT55" s="55"/>
+      <c r="AU55" s="55"/>
+      <c r="AV55" s="55"/>
+      <c r="AW55" s="55"/>
+      <c r="AX55" s="55"/>
+      <c r="AY55" s="55"/>
+      <c r="AZ55" s="55"/>
+      <c r="BA55" s="55"/>
+      <c r="BB55" s="55"/>
+      <c r="BC55" s="55"/>
+      <c r="BD55" s="55"/>
+      <c r="BE55" s="55"/>
+      <c r="BF55" s="55"/>
+      <c r="BG55" s="55"/>
+      <c r="BH55" s="55"/>
+      <c r="BI55" s="55"/>
+      <c r="BJ55" s="55"/>
+      <c r="BK55" s="55"/>
+    </row>
+    <row r="56" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="P2:Y2"/>
+    <mergeCell ref="P1:Y1"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="H2:N2"/>
     <mergeCell ref="BE4:BK4"/>
     <mergeCell ref="H4:N4"/>
     <mergeCell ref="O4:U4"/>
@@ -5507,17 +6047,8 @@
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AQ4:AW4"/>
     <mergeCell ref="AX4:BD4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="P2:Y2"/>
-    <mergeCell ref="P1:Y1"/>
-    <mergeCell ref="H1:N1"/>
-    <mergeCell ref="H2:N2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:C48">
+  <conditionalFormatting sqref="C7:C55">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5531,7 +6062,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:BK42 H44:BK47">
+  <conditionalFormatting sqref="H4:BK49 H51:BK54">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>AND(TODAY()&gt;=H$5, TODAY()&lt;I$5)</formula>
     </cfRule>
@@ -5544,7 +6075,7 @@
       <formula>AND(task_end&gt;=H$5,task_start&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17:BK26">
+  <conditionalFormatting sqref="H17:BK33">
     <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -5552,7 +6083,7 @@
       <formula>AND(task_end&gt;=H$5,task_start&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H28:BK33">
+  <conditionalFormatting sqref="H35:BK40">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -5560,7 +6091,7 @@
       <formula>AND(task_end&gt;=H$5,task_start&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H35:BK42 H44:BK47">
+  <conditionalFormatting sqref="H42:BK49 H51:BK54">
     <cfRule type="expression" dxfId="1" priority="36">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -5581,9 +6112,9 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="B9 contains the task name.  C9 is the assignee.  D9 is a progress bar that shades based on the number entered into the cell.  _x000a__x000a_E9 contains the start date and F9 contains the end date._x000a__x000a_The Gantt chart will fill in starting in cell I9 based on task dates." sqref="A9" xr:uid="{D870A2F6-6B07-4F5A-A81D-4BCCFADF8796}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A10" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A16" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A27" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A34" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A48" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A34" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A41" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A55" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -5596,7 +6127,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="E31 E34 E27" formula="1"/>
+    <ignoredError sqref="E38 E41 E34" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -5614,7 +6145,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C7:C48</xm:sqref>
+          <xm:sqref>C7:C55</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5747,12 +6278,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6068,29 +6610,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6117,13 +6652,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add updated use case diagram and new wireframes
Added UseCaseV3.drawio to reflect updated system use cases. Introduced new wireframes for Analytics, Incidents, Login, Notifications, Settings, and ViewIncidents. Moved previous wireframes to the 'Old' directory for archival. Updated Gannt.xlsx with latest changes.
</commit_message>
<xml_diff>
--- a/Documentation/Gannt.xlsx
+++ b/Documentation/Gannt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Github\Year3\COMP3000-Computing-Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D74F453-9226-461C-97E9-7E6C55E71662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB50C21-316F-426B-B4BF-FFA1C786AF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -1124,15 +1124,19 @@
     <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="16" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="17" fillId="11" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1149,19 +1153,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1762,8 +1762,8 @@
   </sheetPr>
   <dimension ref="A1:BK57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1787,28 +1787,28 @@
       <c r="D1" s="65"/>
       <c r="E1" s="66"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="109" t="s">
+      <c r="H1" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="110"/>
-      <c r="M1" s="110"/>
-      <c r="N1" s="110"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
       <c r="O1" s="16"/>
-      <c r="P1" s="107">
+      <c r="P1" s="109">
         <v>45922</v>
       </c>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
-      <c r="U1" s="108"/>
-      <c r="V1" s="108"/>
-      <c r="W1" s="108"/>
-      <c r="X1" s="108"/>
-      <c r="Y1" s="108"/>
+      <c r="Q1" s="110"/>
+      <c r="R1" s="110"/>
+      <c r="S1" s="110"/>
+      <c r="T1" s="110"/>
+      <c r="U1" s="110"/>
+      <c r="V1" s="110"/>
+      <c r="W1" s="110"/>
+      <c r="X1" s="110"/>
+      <c r="Y1" s="110"/>
     </row>
     <row r="2" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="56" t="s">
@@ -1817,28 +1817,28 @@
       <c r="C2" s="15"/>
       <c r="D2" s="67"/>
       <c r="E2" s="68"/>
-      <c r="H2" s="109" t="s">
+      <c r="H2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110"/>
-      <c r="L2" s="110"/>
-      <c r="M2" s="110"/>
-      <c r="N2" s="110"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="112"/>
+      <c r="N2" s="112"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="105">
+      <c r="P2" s="107">
         <v>3</v>
       </c>
-      <c r="Q2" s="106"/>
-      <c r="R2" s="106"/>
-      <c r="S2" s="106"/>
-      <c r="T2" s="106"/>
-      <c r="U2" s="106"/>
-      <c r="V2" s="106"/>
-      <c r="W2" s="106"/>
-      <c r="X2" s="106"/>
-      <c r="Y2" s="106"/>
+      <c r="Q2" s="108"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="108"/>
+      <c r="T2" s="108"/>
+      <c r="U2" s="108"/>
+      <c r="V2" s="108"/>
+      <c r="W2" s="108"/>
+      <c r="X2" s="108"/>
+      <c r="Y2" s="108"/>
     </row>
     <row r="3" spans="1:63" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
@@ -1856,99 +1856,99 @@
       </c>
       <c r="D4" s="71"/>
       <c r="E4" s="70"/>
-      <c r="H4" s="102">
+      <c r="H4" s="115">
         <f>H5</f>
         <v>45936</v>
       </c>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="100">
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
+      <c r="N4" s="113"/>
+      <c r="O4" s="113">
         <f>O5</f>
         <v>45943</v>
       </c>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
-      <c r="T4" s="100"/>
-      <c r="U4" s="100"/>
-      <c r="V4" s="100">
+      <c r="P4" s="113"/>
+      <c r="Q4" s="113"/>
+      <c r="R4" s="113"/>
+      <c r="S4" s="113"/>
+      <c r="T4" s="113"/>
+      <c r="U4" s="113"/>
+      <c r="V4" s="113">
         <f>V5</f>
         <v>45950</v>
       </c>
-      <c r="W4" s="100"/>
-      <c r="X4" s="100"/>
-      <c r="Y4" s="100"/>
-      <c r="Z4" s="100"/>
-      <c r="AA4" s="100"/>
-      <c r="AB4" s="100"/>
-      <c r="AC4" s="100">
+      <c r="W4" s="113"/>
+      <c r="X4" s="113"/>
+      <c r="Y4" s="113"/>
+      <c r="Z4" s="113"/>
+      <c r="AA4" s="113"/>
+      <c r="AB4" s="113"/>
+      <c r="AC4" s="113">
         <f>AC5</f>
         <v>45957</v>
       </c>
-      <c r="AD4" s="100"/>
-      <c r="AE4" s="100"/>
-      <c r="AF4" s="100"/>
-      <c r="AG4" s="100"/>
-      <c r="AH4" s="100"/>
-      <c r="AI4" s="100"/>
-      <c r="AJ4" s="100">
+      <c r="AD4" s="113"/>
+      <c r="AE4" s="113"/>
+      <c r="AF4" s="113"/>
+      <c r="AG4" s="113"/>
+      <c r="AH4" s="113"/>
+      <c r="AI4" s="113"/>
+      <c r="AJ4" s="113">
         <f>AJ5</f>
         <v>45964</v>
       </c>
-      <c r="AK4" s="100"/>
-      <c r="AL4" s="100"/>
-      <c r="AM4" s="100"/>
-      <c r="AN4" s="100"/>
-      <c r="AO4" s="100"/>
-      <c r="AP4" s="100"/>
-      <c r="AQ4" s="100">
+      <c r="AK4" s="113"/>
+      <c r="AL4" s="113"/>
+      <c r="AM4" s="113"/>
+      <c r="AN4" s="113"/>
+      <c r="AO4" s="113"/>
+      <c r="AP4" s="113"/>
+      <c r="AQ4" s="113">
         <f>AQ5</f>
         <v>45971</v>
       </c>
-      <c r="AR4" s="100"/>
-      <c r="AS4" s="100"/>
-      <c r="AT4" s="100"/>
-      <c r="AU4" s="100"/>
-      <c r="AV4" s="100"/>
-      <c r="AW4" s="100"/>
-      <c r="AX4" s="100">
+      <c r="AR4" s="113"/>
+      <c r="AS4" s="113"/>
+      <c r="AT4" s="113"/>
+      <c r="AU4" s="113"/>
+      <c r="AV4" s="113"/>
+      <c r="AW4" s="113"/>
+      <c r="AX4" s="113">
         <f>AX5</f>
         <v>45978</v>
       </c>
-      <c r="AY4" s="100"/>
-      <c r="AZ4" s="100"/>
-      <c r="BA4" s="100"/>
-      <c r="BB4" s="100"/>
-      <c r="BC4" s="100"/>
-      <c r="BD4" s="100"/>
-      <c r="BE4" s="100">
+      <c r="AY4" s="113"/>
+      <c r="AZ4" s="113"/>
+      <c r="BA4" s="113"/>
+      <c r="BB4" s="113"/>
+      <c r="BC4" s="113"/>
+      <c r="BD4" s="113"/>
+      <c r="BE4" s="113">
         <f>BE5</f>
         <v>45985</v>
       </c>
-      <c r="BF4" s="100"/>
-      <c r="BG4" s="100"/>
-      <c r="BH4" s="100"/>
-      <c r="BI4" s="100"/>
-      <c r="BJ4" s="100"/>
-      <c r="BK4" s="101"/>
+      <c r="BF4" s="113"/>
+      <c r="BG4" s="113"/>
+      <c r="BH4" s="113"/>
+      <c r="BI4" s="113"/>
+      <c r="BJ4" s="113"/>
+      <c r="BK4" s="114"/>
     </row>
     <row r="5" spans="1:63" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="111"/>
-      <c r="B5" s="112" t="s">
+      <c r="A5" s="100"/>
+      <c r="B5" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="114" t="s">
+      <c r="C5" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="103" t="s">
+      <c r="E5" s="105" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="21">
@@ -2177,11 +2177,11 @@
       </c>
     </row>
     <row r="6" spans="1:63" s="18" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="111"/>
-      <c r="B6" s="113"/>
-      <c r="C6" s="115"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
+      <c r="A6" s="100"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="106"/>
       <c r="H6" s="24" t="str">
         <f t="shared" ref="H6:AM6" si="3">LEFT(TEXT(H5,"ddd"),1)</f>
         <v>M</v>
@@ -3115,7 +3115,7 @@
         <v>62</v>
       </c>
       <c r="C17" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="79">
         <v>45968</v>
@@ -3192,7 +3192,7 @@
         <v>63</v>
       </c>
       <c r="C18" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="79">
         <v>45968</v>
@@ -3265,7 +3265,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="79">
         <v>45968</v>
@@ -6030,11 +6030,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
     <mergeCell ref="P2:Y2"/>
     <mergeCell ref="P1:Y1"/>
     <mergeCell ref="H1:N1"/>
@@ -6047,6 +6042,11 @@
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AQ4:AW4"/>
     <mergeCell ref="AX4:BD4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C55">
     <cfRule type="dataBar" priority="23">
@@ -6298,6 +6298,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6609,15 +6618,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
@@ -6631,6 +6631,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6651,14 +6659,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>